<commit_message>
updated test script for  admin module
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B66EEE0E-7793-4D98-9BEE-A78371A6E345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\GUIFramework\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA950FB-FECC-4B75-B88E-38CF1AA0B81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11620" windowHeight="6330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
     <sheet name="org" sheetId="1" r:id="rId2"/>
     <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="alpha" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="177">
   <si>
     <t>TC_ID</t>
   </si>
@@ -444,13 +449,124 @@
   </si>
   <si>
     <t>faceBook_kdd</t>
+  </si>
+  <si>
+    <t>No of stock to increase</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>No of stock to decrease</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Basketball</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>No.of stocks</t>
+  </si>
+  <si>
+    <t>woodland</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>woodlandbrown</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>sparkRed</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>spark</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>expectedBasketballpagetitle</t>
+  </si>
+  <si>
+    <t>expectedAddproductpagetitle</t>
+  </si>
+  <si>
+    <t>Transcations</t>
+  </si>
+  <si>
+    <t>expectedtranscactionspagetitle</t>
+  </si>
+  <si>
+    <t>expectedReceiptpage</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>Official Receipt</t>
+  </si>
+  <si>
+    <t>StockINProductINFeatureTest</t>
+  </si>
+  <si>
+    <t>expectedfeaturespagetitle</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>expectedStockinpagetitle</t>
+  </si>
+  <si>
+    <t>Stock IN</t>
+  </si>
+  <si>
+    <t>StockINProductOUTFeatureTest</t>
+  </si>
+  <si>
+    <t>expectedStockoutpagetitle</t>
+  </si>
+  <si>
+    <t>Stock OUT</t>
+  </si>
+  <si>
+    <t>expectedFootballtitlepage</t>
+  </si>
+  <si>
+    <t>Add Product...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,8 +574,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +601,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,13 +649,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,15 +947,15 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +970,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -840,14 +983,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +1005,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -875,14 +1018,14 @@
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +1042,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>127</v>
       </c>
@@ -923,18 +1066,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +1090,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -960,7 +1103,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,7 +1120,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>110</v>
       </c>
@@ -994,7 +1137,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1151,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -1022,7 +1165,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1177,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>115</v>
       </c>
@@ -1059,13 +1202,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -1073,7 +1216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>135</v>
       </c>
@@ -1081,7 +1224,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>135</v>
       </c>
@@ -1089,7 +1232,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
@@ -1103,6 +1246,210 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95230730-14BB-4006-A554-3380205AFB6A}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
   <dimension ref="A1:B100"/>
   <sheetViews>
@@ -1110,13 +1457,13 @@
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,7 +1471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1212,7 +1559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1220,7 +1567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1276,7 +1623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1663,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1671,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1687,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1695,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1703,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1711,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1719,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1727,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1388,7 +1735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -1396,7 +1743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -1412,7 +1759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +1767,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -1428,7 +1775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -1436,7 +1783,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1799,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1807,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1815,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1476,7 +1823,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -1484,7 +1831,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -1492,7 +1839,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1847,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1855,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1863,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>58</v>
       </c>
@@ -1524,7 +1871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>58</v>
       </c>
@@ -1532,7 +1879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -1540,7 +1887,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>58</v>
       </c>
@@ -1548,7 +1895,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -1556,7 +1903,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -1564,7 +1911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -1572,7 +1919,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -1580,7 +1927,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
@@ -1596,7 +1943,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1604,7 +1951,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
@@ -1612,7 +1959,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
@@ -1628,7 +1975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
@@ -1636,7 +1983,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>58</v>
       </c>
@@ -1644,7 +1991,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
@@ -1652,7 +1999,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>58</v>
       </c>
@@ -1660,7 +2007,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>58</v>
       </c>
@@ -1668,7 +2015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>58</v>
       </c>
@@ -1676,7 +2023,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>58</v>
       </c>
@@ -1684,7 +2031,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>58</v>
       </c>
@@ -1692,7 +2039,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>58</v>
       </c>
@@ -1700,7 +2047,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>58</v>
       </c>
@@ -1708,7 +2055,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
@@ -1716,7 +2063,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>58</v>
       </c>
@@ -1724,7 +2071,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>58</v>
       </c>
@@ -1732,7 +2079,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>58</v>
       </c>
@@ -1740,7 +2087,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +2095,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>58</v>
       </c>
@@ -1756,7 +2103,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>58</v>
       </c>
@@ -1764,7 +2111,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>58</v>
       </c>
@@ -1772,7 +2119,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
@@ -1780,7 +2127,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>58</v>
       </c>
@@ -1788,7 +2135,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>58</v>
       </c>
@@ -1796,7 +2143,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>58</v>
       </c>
@@ -1804,7 +2151,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +2159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>58</v>
       </c>
@@ -1820,7 +2167,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +2175,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>58</v>
       </c>
@@ -1836,7 +2183,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +2191,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>58</v>
       </c>
@@ -1852,7 +2199,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>58</v>
       </c>
@@ -1860,7 +2207,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>58</v>
       </c>
@@ -1868,7 +2215,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>58</v>
       </c>
@@ -1876,7 +2223,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>58</v>
       </c>
@@ -1884,7 +2231,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>58</v>
       </c>
@@ -1892,7 +2239,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -1900,7 +2247,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>58</v>
       </c>
@@ -1908,7 +2255,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>